<commit_message>
added another test record
</commit_message>
<xml_diff>
--- a/data/20221116_excel_example.xlsx
+++ b/data/20221116_excel_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwroberts\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wainr\OneDrive\Documents\xlsx_to_xml_endnote\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D1B9B0-2B56-48C9-A51F-D708BB64CAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2011670-92EF-45E6-8F9B-16EB8D4095EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32505" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="293">
   <si>
     <t>ID</t>
   </si>
@@ -916,6 +916,9 @@
   </si>
   <si>
     <t>Morrilton, AR</t>
+  </si>
+  <si>
+    <t>another title</t>
   </si>
 </sst>
 </file>
@@ -968,22 +971,6 @@
   </cellStyles>
   <dxfs count="159">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -2389,6 +2376,22 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2410,166 +2413,166 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:FA12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:FA12" totalsRowShown="0" headerRowDxfId="158" dataDxfId="157">
   <autoFilter ref="A1:FA12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="157">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="158"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="157"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completion time" dataDxfId="156"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="155"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="154"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reference Type" dataDxfId="153"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Title" dataDxfId="152"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Author(s)" dataDxfId="151"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Year" dataDxfId="150"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Attach files (i.e., pdf, photograph)" dataDxfId="149"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Where did the research take place/what is the location of the reference?" dataDxfId="148"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Reference description" dataDxfId="147"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Cover and/or forest type" dataDxfId="146"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Stable URL or DOI" dataDxfId="145"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Title2" dataDxfId="144"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Photographer(s)" dataDxfId="143"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Year2" dataDxfId="142"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Is this photograph in the public domain?" dataDxfId="141"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Attach files (i.e., pdf, photograph)2" dataDxfId="140"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Where did the research take place/what is the location of the reference?2" dataDxfId="139"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Photograph caption" dataDxfId="138"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Cover and/or forest type2" dataDxfId="137"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Stable URL or DOI2" dataDxfId="136"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Title3" dataDxfId="135"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Cartographer(s)" dataDxfId="134"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Year3" dataDxfId="133"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Date, if month or day is known." dataDxfId="132"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Attach files (i.e., pdf, photograph)3" dataDxfId="131"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Where did the research take place/what is the location of the reference?3" dataDxfId="130"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Map description" dataDxfId="129"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Cover and/or forest type3" dataDxfId="128"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Stable URL or DOI3" dataDxfId="127"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Title4" dataDxfId="126"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Author(s)2" dataDxfId="125"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Year4" dataDxfId="124"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Journal (name of periodical)" dataDxfId="123"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Volume" dataDxfId="122"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Issue" dataDxfId="121"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Page Range" dataDxfId="120"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Attach files (i.e., pdf, photograph)4" dataDxfId="119"/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Where did the research take place/what is the location of the reference?4" dataDxfId="118"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Reference description2" dataDxfId="117"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Cover and/or forest type4" dataDxfId="116"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Stable URL or DOI4" dataDxfId="115"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Title5" dataDxfId="114"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Author(s)3" dataDxfId="113"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Year5" dataDxfId="112"/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Series Editor" dataDxfId="111"/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Series Title" dataDxfId="110"/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Place Published" dataDxfId="109"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Institution" dataDxfId="108"/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Volume2" dataDxfId="107"/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Series Volume" dataDxfId="106"/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="Document Number" dataDxfId="105"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="Number of Pages" dataDxfId="104"/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="Publisher" dataDxfId="103"/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="Edition" dataDxfId="102"/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="Attach files (i.e., pdf, photograph)5" dataDxfId="101"/>
-    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="Reference description3" dataDxfId="100"/>
-    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="Where did the research take place/what is the location of the reference?5" dataDxfId="99"/>
-    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="Cover and/or forest type5" dataDxfId="98"/>
-    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="Stable URL or DOI5" dataDxfId="97"/>
-    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="Title6" dataDxfId="96"/>
-    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="Author(s)4" dataDxfId="95"/>
-    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="Year6" dataDxfId="94"/>
-    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="Attach files (i.e., pdf, photograph)6" dataDxfId="93"/>
-    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="Where did the research take place/what is the location of the reference?6" dataDxfId="92"/>
-    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="Reference description4" dataDxfId="91"/>
-    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="Cover and/or forest type6" dataDxfId="90"/>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="Stable URL or DOI6" dataDxfId="89"/>
-    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="Number of Volumes" dataDxfId="88"/>
-    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="Series editor2" dataDxfId="87"/>
-    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" name="Series title2" dataDxfId="86"/>
-    <tableColumn id="74" xr3:uid="{00000000-0010-0000-0000-00004A000000}" name="Edition2" dataDxfId="85"/>
-    <tableColumn id="75" xr3:uid="{00000000-0010-0000-0000-00004B000000}" name="Title7" dataDxfId="84"/>
-    <tableColumn id="76" xr3:uid="{00000000-0010-0000-0000-00004C000000}" name="Author(s)5" dataDxfId="83"/>
-    <tableColumn id="77" xr3:uid="{00000000-0010-0000-0000-00004D000000}" name="Year7" dataDxfId="82"/>
-    <tableColumn id="78" xr3:uid="{00000000-0010-0000-0000-00004E000000}" name="Attach files (i.e., pdf, photograph)7" dataDxfId="81"/>
-    <tableColumn id="79" xr3:uid="{00000000-0010-0000-0000-00004F000000}" name="Where did the research take place/what is the location of the reference?7" dataDxfId="80"/>
-    <tableColumn id="80" xr3:uid="{00000000-0010-0000-0000-000050000000}" name="Reference description5" dataDxfId="79"/>
-    <tableColumn id="81" xr3:uid="{00000000-0010-0000-0000-000051000000}" name="Cover and/or forest type7" dataDxfId="78"/>
-    <tableColumn id="82" xr3:uid="{00000000-0010-0000-0000-000052000000}" name="Stable URL or DOI7" dataDxfId="77"/>
-    <tableColumn id="83" xr3:uid="{00000000-0010-0000-0000-000053000000}" name="Session" dataDxfId="76"/>
-    <tableColumn id="84" xr3:uid="{00000000-0010-0000-0000-000054000000}" name="Paper Number" dataDxfId="75"/>
-    <tableColumn id="85" xr3:uid="{00000000-0010-0000-0000-000055000000}" name="Editor" dataDxfId="74"/>
-    <tableColumn id="86" xr3:uid="{00000000-0010-0000-0000-000056000000}" name="Conference name" dataDxfId="73"/>
-    <tableColumn id="87" xr3:uid="{00000000-0010-0000-0000-000057000000}" name="Conference location" dataDxfId="72"/>
-    <tableColumn id="88" xr3:uid="{00000000-0010-0000-0000-000058000000}" name="Publisher2" dataDxfId="71"/>
-    <tableColumn id="89" xr3:uid="{00000000-0010-0000-0000-000059000000}" name="Volume3" dataDxfId="70"/>
-    <tableColumn id="90" xr3:uid="{00000000-0010-0000-0000-00005A000000}" name="Issue2" dataDxfId="69"/>
-    <tableColumn id="91" xr3:uid="{00000000-0010-0000-0000-00005B000000}" name="Page Range2" dataDxfId="68"/>
-    <tableColumn id="92" xr3:uid="{00000000-0010-0000-0000-00005C000000}" name="Title8" dataDxfId="67"/>
-    <tableColumn id="93" xr3:uid="{00000000-0010-0000-0000-00005D000000}" name="Author(s)6" dataDxfId="66"/>
-    <tableColumn id="94" xr3:uid="{00000000-0010-0000-0000-00005E000000}" name="Year8" dataDxfId="65"/>
-    <tableColumn id="95" xr3:uid="{00000000-0010-0000-0000-00005F000000}" name="Attach files (i.e., pdf, photograph)8" dataDxfId="64"/>
-    <tableColumn id="96" xr3:uid="{00000000-0010-0000-0000-000060000000}" name="Where did the research take place/what is the location of the reference?8" dataDxfId="63"/>
-    <tableColumn id="97" xr3:uid="{00000000-0010-0000-0000-000061000000}" name="Reference description6" dataDxfId="62"/>
-    <tableColumn id="98" xr3:uid="{00000000-0010-0000-0000-000062000000}" name="Cover and/or forest type8" dataDxfId="61"/>
-    <tableColumn id="99" xr3:uid="{00000000-0010-0000-0000-000063000000}" name="Stable URL or DOI8" dataDxfId="60"/>
-    <tableColumn id="100" xr3:uid="{00000000-0010-0000-0000-000064000000}" name="Academic Department" dataDxfId="59"/>
-    <tableColumn id="101" xr3:uid="{00000000-0010-0000-0000-000065000000}" name="University" dataDxfId="58"/>
-    <tableColumn id="102" xr3:uid="{00000000-0010-0000-0000-000066000000}" name="Degree" dataDxfId="57"/>
-    <tableColumn id="103" xr3:uid="{00000000-0010-0000-0000-000067000000}" name="Place Published2" dataDxfId="56"/>
-    <tableColumn id="104" xr3:uid="{00000000-0010-0000-0000-000068000000}" name="Number of pages2" dataDxfId="55"/>
-    <tableColumn id="105" xr3:uid="{00000000-0010-0000-0000-000069000000}" name="Title9" dataDxfId="54"/>
-    <tableColumn id="106" xr3:uid="{00000000-0010-0000-0000-00006A000000}" name="Author(s)7" dataDxfId="53"/>
-    <tableColumn id="107" xr3:uid="{00000000-0010-0000-0000-00006B000000}" name="Year9" dataDxfId="52"/>
-    <tableColumn id="108" xr3:uid="{00000000-0010-0000-0000-00006C000000}" name="Edition3" dataDxfId="51"/>
-    <tableColumn id="109" xr3:uid="{00000000-0010-0000-0000-00006D000000}" name="Editor2" dataDxfId="50"/>
-    <tableColumn id="110" xr3:uid="{00000000-0010-0000-0000-00006E000000}" name="Number of Volumes2" dataDxfId="49"/>
-    <tableColumn id="111" xr3:uid="{00000000-0010-0000-0000-00006F000000}" name="Series Volume2" dataDxfId="48"/>
-    <tableColumn id="112" xr3:uid="{00000000-0010-0000-0000-000070000000}" name="Place Published3" dataDxfId="47"/>
-    <tableColumn id="113" xr3:uid="{00000000-0010-0000-0000-000071000000}" name="Publisher3" dataDxfId="46"/>
-    <tableColumn id="114" xr3:uid="{00000000-0010-0000-0000-000072000000}" name="Volume4" dataDxfId="45"/>
-    <tableColumn id="115" xr3:uid="{00000000-0010-0000-0000-000073000000}" name="Series Editor3" dataDxfId="44"/>
-    <tableColumn id="116" xr3:uid="{00000000-0010-0000-0000-000074000000}" name="Series Title3" dataDxfId="43"/>
-    <tableColumn id="117" xr3:uid="{00000000-0010-0000-0000-000075000000}" name="Attach files (i.e., pdf, photograph)9" dataDxfId="42"/>
-    <tableColumn id="118" xr3:uid="{00000000-0010-0000-0000-000076000000}" name="Where did the research take place/what is the location of the reference?9" dataDxfId="41"/>
-    <tableColumn id="119" xr3:uid="{00000000-0010-0000-0000-000077000000}" name="Reference description7" dataDxfId="40"/>
-    <tableColumn id="120" xr3:uid="{00000000-0010-0000-0000-000078000000}" name="Cover and/or forest type9" dataDxfId="39"/>
-    <tableColumn id="121" xr3:uid="{00000000-0010-0000-0000-000079000000}" name="Stable URL or DOI9" dataDxfId="38"/>
-    <tableColumn id="122" xr3:uid="{00000000-0010-0000-0000-00007A000000}" name="Number of Pages3" dataDxfId="37"/>
-    <tableColumn id="123" xr3:uid="{00000000-0010-0000-0000-00007B000000}" name="Title10" dataDxfId="36"/>
-    <tableColumn id="124" xr3:uid="{00000000-0010-0000-0000-00007C000000}" name="Book Title" dataDxfId="35"/>
-    <tableColumn id="125" xr3:uid="{00000000-0010-0000-0000-00007D000000}" name="Author(s)8" dataDxfId="34"/>
-    <tableColumn id="126" xr3:uid="{00000000-0010-0000-0000-00007E000000}" name="Year10" dataDxfId="33"/>
-    <tableColumn id="127" xr3:uid="{00000000-0010-0000-0000-00007F000000}" name="Edition4" dataDxfId="32"/>
-    <tableColumn id="128" xr3:uid="{00000000-0010-0000-0000-000080000000}" name="Editor3" dataDxfId="31"/>
-    <tableColumn id="129" xr3:uid="{00000000-0010-0000-0000-000081000000}" name="Number of Volumes3" dataDxfId="30"/>
-    <tableColumn id="130" xr3:uid="{00000000-0010-0000-0000-000082000000}" name="Series Volume3" dataDxfId="29"/>
-    <tableColumn id="131" xr3:uid="{00000000-0010-0000-0000-000083000000}" name="Place Published4" dataDxfId="28"/>
-    <tableColumn id="132" xr3:uid="{00000000-0010-0000-0000-000084000000}" name="Publisher4" dataDxfId="27"/>
-    <tableColumn id="133" xr3:uid="{00000000-0010-0000-0000-000085000000}" name="Volume5" dataDxfId="26"/>
-    <tableColumn id="134" xr3:uid="{00000000-0010-0000-0000-000086000000}" name="Series Editor4" dataDxfId="25"/>
-    <tableColumn id="135" xr3:uid="{00000000-0010-0000-0000-000087000000}" name="Series Title4" dataDxfId="24"/>
-    <tableColumn id="136" xr3:uid="{00000000-0010-0000-0000-000088000000}" name="Page Range3" dataDxfId="23"/>
-    <tableColumn id="137" xr3:uid="{00000000-0010-0000-0000-000089000000}" name="Chapter Number" dataDxfId="22"/>
-    <tableColumn id="138" xr3:uid="{00000000-0010-0000-0000-00008A000000}" name="Attach files (i.e., pdf, photograph)10" dataDxfId="21"/>
-    <tableColumn id="139" xr3:uid="{00000000-0010-0000-0000-00008B000000}" name="Where did the research take place/what is the location of the reference?10" dataDxfId="20"/>
-    <tableColumn id="140" xr3:uid="{00000000-0010-0000-0000-00008C000000}" name="Reference description8" dataDxfId="19"/>
-    <tableColumn id="141" xr3:uid="{00000000-0010-0000-0000-00008D000000}" name="Cover and/or forest type10" dataDxfId="18"/>
-    <tableColumn id="142" xr3:uid="{00000000-0010-0000-0000-00008E000000}" name="Stable URL or DOI10" dataDxfId="17"/>
-    <tableColumn id="143" xr3:uid="{00000000-0010-0000-0000-00008F000000}" name="Title11" dataDxfId="16"/>
-    <tableColumn id="144" xr3:uid="{00000000-0010-0000-0000-000090000000}" name="Author(s)/Reporter(s)" dataDxfId="15"/>
-    <tableColumn id="145" xr3:uid="{00000000-0010-0000-0000-000091000000}" name="Year11" dataDxfId="14"/>
-    <tableColumn id="146" xr3:uid="{00000000-0010-0000-0000-000092000000}" name="Newspaper" dataDxfId="13"/>
-    <tableColumn id="147" xr3:uid="{00000000-0010-0000-0000-000093000000}" name="Attach files (i.e., pdf, photograph)11" dataDxfId="12"/>
-    <tableColumn id="148" xr3:uid="{00000000-0010-0000-0000-000094000000}" name="Where did the research take place/what is the location of the reference?11" dataDxfId="11"/>
-    <tableColumn id="149" xr3:uid="{00000000-0010-0000-0000-000095000000}" name="Reference description9" dataDxfId="10"/>
-    <tableColumn id="150" xr3:uid="{00000000-0010-0000-0000-000096000000}" name="Cover and/or forest type11" dataDxfId="9"/>
-    <tableColumn id="151" xr3:uid="{00000000-0010-0000-0000-000097000000}" name="Stable URL or DOI11" dataDxfId="8"/>
-    <tableColumn id="152" xr3:uid="{00000000-0010-0000-0000-000098000000}" name="Place published5" dataDxfId="7"/>
-    <tableColumn id="153" xr3:uid="{00000000-0010-0000-0000-000099000000}" name="Publisher5" dataDxfId="6"/>
-    <tableColumn id="154" xr3:uid="{00000000-0010-0000-0000-00009A000000}" name="Page Range4" dataDxfId="5"/>
-    <tableColumn id="155" xr3:uid="{00000000-0010-0000-0000-00009B000000}" name="Volume6" dataDxfId="4"/>
-    <tableColumn id="156" xr3:uid="{00000000-0010-0000-0000-00009C000000}" name="Edition5" dataDxfId="3"/>
-    <tableColumn id="157" xr3:uid="{00000000-0010-0000-0000-00009D000000}" name="Section" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="156"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="155"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completion time" dataDxfId="154"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="153"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="152"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Reference Type" dataDxfId="151"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Title" dataDxfId="150"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Author(s)" dataDxfId="149"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Year" dataDxfId="148"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Attach files (i.e., pdf, photograph)" dataDxfId="147"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Where did the research take place/what is the location of the reference?" dataDxfId="146"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Reference description" dataDxfId="145"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Cover and/or forest type" dataDxfId="144"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Stable URL or DOI" dataDxfId="143"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Title2" dataDxfId="142"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Photographer(s)" dataDxfId="141"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Year2" dataDxfId="140"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Is this photograph in the public domain?" dataDxfId="139"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Attach files (i.e., pdf, photograph)2" dataDxfId="138"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Where did the research take place/what is the location of the reference?2" dataDxfId="137"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Photograph caption" dataDxfId="136"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Cover and/or forest type2" dataDxfId="135"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Stable URL or DOI2" dataDxfId="134"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Title3" dataDxfId="133"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Cartographer(s)" dataDxfId="132"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Year3" dataDxfId="131"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Date, if month or day is known." dataDxfId="130"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Attach files (i.e., pdf, photograph)3" dataDxfId="129"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Where did the research take place/what is the location of the reference?3" dataDxfId="128"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Map description" dataDxfId="127"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Cover and/or forest type3" dataDxfId="126"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Stable URL or DOI3" dataDxfId="125"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Title4" dataDxfId="124"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Author(s)2" dataDxfId="123"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Year4" dataDxfId="122"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Journal (name of periodical)" dataDxfId="121"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Volume" dataDxfId="120"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Issue" dataDxfId="119"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Page Range" dataDxfId="118"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Attach files (i.e., pdf, photograph)4" dataDxfId="117"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Where did the research take place/what is the location of the reference?4" dataDxfId="116"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Reference description2" dataDxfId="115"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Cover and/or forest type4" dataDxfId="114"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Stable URL or DOI4" dataDxfId="113"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Title5" dataDxfId="112"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Author(s)3" dataDxfId="111"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Year5" dataDxfId="110"/>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Series Editor" dataDxfId="109"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Series Title" dataDxfId="108"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Place Published" dataDxfId="107"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Institution" dataDxfId="106"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Volume2" dataDxfId="105"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Series Volume" dataDxfId="104"/>
+    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="Document Number" dataDxfId="103"/>
+    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="Number of Pages" dataDxfId="102"/>
+    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="Publisher" dataDxfId="101"/>
+    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="Edition" dataDxfId="100"/>
+    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="Attach files (i.e., pdf, photograph)5" dataDxfId="99"/>
+    <tableColumn id="59" xr3:uid="{00000000-0010-0000-0000-00003B000000}" name="Reference description3" dataDxfId="98"/>
+    <tableColumn id="60" xr3:uid="{00000000-0010-0000-0000-00003C000000}" name="Where did the research take place/what is the location of the reference?5" dataDxfId="97"/>
+    <tableColumn id="61" xr3:uid="{00000000-0010-0000-0000-00003D000000}" name="Cover and/or forest type5" dataDxfId="96"/>
+    <tableColumn id="62" xr3:uid="{00000000-0010-0000-0000-00003E000000}" name="Stable URL or DOI5" dataDxfId="95"/>
+    <tableColumn id="63" xr3:uid="{00000000-0010-0000-0000-00003F000000}" name="Title6" dataDxfId="94"/>
+    <tableColumn id="64" xr3:uid="{00000000-0010-0000-0000-000040000000}" name="Author(s)4" dataDxfId="93"/>
+    <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="Year6" dataDxfId="92"/>
+    <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="Attach files (i.e., pdf, photograph)6" dataDxfId="91"/>
+    <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="Where did the research take place/what is the location of the reference?6" dataDxfId="90"/>
+    <tableColumn id="68" xr3:uid="{00000000-0010-0000-0000-000044000000}" name="Reference description4" dataDxfId="89"/>
+    <tableColumn id="69" xr3:uid="{00000000-0010-0000-0000-000045000000}" name="Cover and/or forest type6" dataDxfId="88"/>
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="Stable URL or DOI6" dataDxfId="87"/>
+    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="Number of Volumes" dataDxfId="86"/>
+    <tableColumn id="72" xr3:uid="{00000000-0010-0000-0000-000048000000}" name="Series editor2" dataDxfId="85"/>
+    <tableColumn id="73" xr3:uid="{00000000-0010-0000-0000-000049000000}" name="Series title2" dataDxfId="84"/>
+    <tableColumn id="74" xr3:uid="{00000000-0010-0000-0000-00004A000000}" name="Edition2" dataDxfId="83"/>
+    <tableColumn id="75" xr3:uid="{00000000-0010-0000-0000-00004B000000}" name="Title7" dataDxfId="82"/>
+    <tableColumn id="76" xr3:uid="{00000000-0010-0000-0000-00004C000000}" name="Author(s)5" dataDxfId="81"/>
+    <tableColumn id="77" xr3:uid="{00000000-0010-0000-0000-00004D000000}" name="Year7" dataDxfId="80"/>
+    <tableColumn id="78" xr3:uid="{00000000-0010-0000-0000-00004E000000}" name="Attach files (i.e., pdf, photograph)7" dataDxfId="79"/>
+    <tableColumn id="79" xr3:uid="{00000000-0010-0000-0000-00004F000000}" name="Where did the research take place/what is the location of the reference?7" dataDxfId="78"/>
+    <tableColumn id="80" xr3:uid="{00000000-0010-0000-0000-000050000000}" name="Reference description5" dataDxfId="77"/>
+    <tableColumn id="81" xr3:uid="{00000000-0010-0000-0000-000051000000}" name="Cover and/or forest type7" dataDxfId="76"/>
+    <tableColumn id="82" xr3:uid="{00000000-0010-0000-0000-000052000000}" name="Stable URL or DOI7" dataDxfId="75"/>
+    <tableColumn id="83" xr3:uid="{00000000-0010-0000-0000-000053000000}" name="Session" dataDxfId="74"/>
+    <tableColumn id="84" xr3:uid="{00000000-0010-0000-0000-000054000000}" name="Paper Number" dataDxfId="73"/>
+    <tableColumn id="85" xr3:uid="{00000000-0010-0000-0000-000055000000}" name="Editor" dataDxfId="72"/>
+    <tableColumn id="86" xr3:uid="{00000000-0010-0000-0000-000056000000}" name="Conference name" dataDxfId="71"/>
+    <tableColumn id="87" xr3:uid="{00000000-0010-0000-0000-000057000000}" name="Conference location" dataDxfId="70"/>
+    <tableColumn id="88" xr3:uid="{00000000-0010-0000-0000-000058000000}" name="Publisher2" dataDxfId="69"/>
+    <tableColumn id="89" xr3:uid="{00000000-0010-0000-0000-000059000000}" name="Volume3" dataDxfId="68"/>
+    <tableColumn id="90" xr3:uid="{00000000-0010-0000-0000-00005A000000}" name="Issue2" dataDxfId="67"/>
+    <tableColumn id="91" xr3:uid="{00000000-0010-0000-0000-00005B000000}" name="Page Range2" dataDxfId="66"/>
+    <tableColumn id="92" xr3:uid="{00000000-0010-0000-0000-00005C000000}" name="Title8" dataDxfId="65"/>
+    <tableColumn id="93" xr3:uid="{00000000-0010-0000-0000-00005D000000}" name="Author(s)6" dataDxfId="64"/>
+    <tableColumn id="94" xr3:uid="{00000000-0010-0000-0000-00005E000000}" name="Year8" dataDxfId="63"/>
+    <tableColumn id="95" xr3:uid="{00000000-0010-0000-0000-00005F000000}" name="Attach files (i.e., pdf, photograph)8" dataDxfId="62"/>
+    <tableColumn id="96" xr3:uid="{00000000-0010-0000-0000-000060000000}" name="Where did the research take place/what is the location of the reference?8" dataDxfId="61"/>
+    <tableColumn id="97" xr3:uid="{00000000-0010-0000-0000-000061000000}" name="Reference description6" dataDxfId="60"/>
+    <tableColumn id="98" xr3:uid="{00000000-0010-0000-0000-000062000000}" name="Cover and/or forest type8" dataDxfId="59"/>
+    <tableColumn id="99" xr3:uid="{00000000-0010-0000-0000-000063000000}" name="Stable URL or DOI8" dataDxfId="58"/>
+    <tableColumn id="100" xr3:uid="{00000000-0010-0000-0000-000064000000}" name="Academic Department" dataDxfId="57"/>
+    <tableColumn id="101" xr3:uid="{00000000-0010-0000-0000-000065000000}" name="University" dataDxfId="56"/>
+    <tableColumn id="102" xr3:uid="{00000000-0010-0000-0000-000066000000}" name="Degree" dataDxfId="55"/>
+    <tableColumn id="103" xr3:uid="{00000000-0010-0000-0000-000067000000}" name="Place Published2" dataDxfId="54"/>
+    <tableColumn id="104" xr3:uid="{00000000-0010-0000-0000-000068000000}" name="Number of pages2" dataDxfId="53"/>
+    <tableColumn id="105" xr3:uid="{00000000-0010-0000-0000-000069000000}" name="Title9" dataDxfId="52"/>
+    <tableColumn id="106" xr3:uid="{00000000-0010-0000-0000-00006A000000}" name="Author(s)7" dataDxfId="51"/>
+    <tableColumn id="107" xr3:uid="{00000000-0010-0000-0000-00006B000000}" name="Year9" dataDxfId="50"/>
+    <tableColumn id="108" xr3:uid="{00000000-0010-0000-0000-00006C000000}" name="Edition3" dataDxfId="49"/>
+    <tableColumn id="109" xr3:uid="{00000000-0010-0000-0000-00006D000000}" name="Editor2" dataDxfId="48"/>
+    <tableColumn id="110" xr3:uid="{00000000-0010-0000-0000-00006E000000}" name="Number of Volumes2" dataDxfId="47"/>
+    <tableColumn id="111" xr3:uid="{00000000-0010-0000-0000-00006F000000}" name="Series Volume2" dataDxfId="46"/>
+    <tableColumn id="112" xr3:uid="{00000000-0010-0000-0000-000070000000}" name="Place Published3" dataDxfId="45"/>
+    <tableColumn id="113" xr3:uid="{00000000-0010-0000-0000-000071000000}" name="Publisher3" dataDxfId="44"/>
+    <tableColumn id="114" xr3:uid="{00000000-0010-0000-0000-000072000000}" name="Volume4" dataDxfId="43"/>
+    <tableColumn id="115" xr3:uid="{00000000-0010-0000-0000-000073000000}" name="Series Editor3" dataDxfId="42"/>
+    <tableColumn id="116" xr3:uid="{00000000-0010-0000-0000-000074000000}" name="Series Title3" dataDxfId="41"/>
+    <tableColumn id="117" xr3:uid="{00000000-0010-0000-0000-000075000000}" name="Attach files (i.e., pdf, photograph)9" dataDxfId="40"/>
+    <tableColumn id="118" xr3:uid="{00000000-0010-0000-0000-000076000000}" name="Where did the research take place/what is the location of the reference?9" dataDxfId="39"/>
+    <tableColumn id="119" xr3:uid="{00000000-0010-0000-0000-000077000000}" name="Reference description7" dataDxfId="38"/>
+    <tableColumn id="120" xr3:uid="{00000000-0010-0000-0000-000078000000}" name="Cover and/or forest type9" dataDxfId="37"/>
+    <tableColumn id="121" xr3:uid="{00000000-0010-0000-0000-000079000000}" name="Stable URL or DOI9" dataDxfId="36"/>
+    <tableColumn id="122" xr3:uid="{00000000-0010-0000-0000-00007A000000}" name="Number of Pages3" dataDxfId="35"/>
+    <tableColumn id="123" xr3:uid="{00000000-0010-0000-0000-00007B000000}" name="Title10" dataDxfId="34"/>
+    <tableColumn id="124" xr3:uid="{00000000-0010-0000-0000-00007C000000}" name="Book Title" dataDxfId="33"/>
+    <tableColumn id="125" xr3:uid="{00000000-0010-0000-0000-00007D000000}" name="Author(s)8" dataDxfId="32"/>
+    <tableColumn id="126" xr3:uid="{00000000-0010-0000-0000-00007E000000}" name="Year10" dataDxfId="31"/>
+    <tableColumn id="127" xr3:uid="{00000000-0010-0000-0000-00007F000000}" name="Edition4" dataDxfId="30"/>
+    <tableColumn id="128" xr3:uid="{00000000-0010-0000-0000-000080000000}" name="Editor3" dataDxfId="29"/>
+    <tableColumn id="129" xr3:uid="{00000000-0010-0000-0000-000081000000}" name="Number of Volumes3" dataDxfId="28"/>
+    <tableColumn id="130" xr3:uid="{00000000-0010-0000-0000-000082000000}" name="Series Volume3" dataDxfId="27"/>
+    <tableColumn id="131" xr3:uid="{00000000-0010-0000-0000-000083000000}" name="Place Published4" dataDxfId="26"/>
+    <tableColumn id="132" xr3:uid="{00000000-0010-0000-0000-000084000000}" name="Publisher4" dataDxfId="25"/>
+    <tableColumn id="133" xr3:uid="{00000000-0010-0000-0000-000085000000}" name="Volume5" dataDxfId="24"/>
+    <tableColumn id="134" xr3:uid="{00000000-0010-0000-0000-000086000000}" name="Series Editor4" dataDxfId="23"/>
+    <tableColumn id="135" xr3:uid="{00000000-0010-0000-0000-000087000000}" name="Series Title4" dataDxfId="22"/>
+    <tableColumn id="136" xr3:uid="{00000000-0010-0000-0000-000088000000}" name="Page Range3" dataDxfId="21"/>
+    <tableColumn id="137" xr3:uid="{00000000-0010-0000-0000-000089000000}" name="Chapter Number" dataDxfId="20"/>
+    <tableColumn id="138" xr3:uid="{00000000-0010-0000-0000-00008A000000}" name="Attach files (i.e., pdf, photograph)10" dataDxfId="19"/>
+    <tableColumn id="139" xr3:uid="{00000000-0010-0000-0000-00008B000000}" name="Where did the research take place/what is the location of the reference?10" dataDxfId="18"/>
+    <tableColumn id="140" xr3:uid="{00000000-0010-0000-0000-00008C000000}" name="Reference description8" dataDxfId="17"/>
+    <tableColumn id="141" xr3:uid="{00000000-0010-0000-0000-00008D000000}" name="Cover and/or forest type10" dataDxfId="16"/>
+    <tableColumn id="142" xr3:uid="{00000000-0010-0000-0000-00008E000000}" name="Stable URL or DOI10" dataDxfId="15"/>
+    <tableColumn id="143" xr3:uid="{00000000-0010-0000-0000-00008F000000}" name="Title11" dataDxfId="14"/>
+    <tableColumn id="144" xr3:uid="{00000000-0010-0000-0000-000090000000}" name="Author(s)/Reporter(s)" dataDxfId="13"/>
+    <tableColumn id="145" xr3:uid="{00000000-0010-0000-0000-000091000000}" name="Year11" dataDxfId="12"/>
+    <tableColumn id="146" xr3:uid="{00000000-0010-0000-0000-000092000000}" name="Newspaper" dataDxfId="11"/>
+    <tableColumn id="147" xr3:uid="{00000000-0010-0000-0000-000093000000}" name="Attach files (i.e., pdf, photograph)11" dataDxfId="10"/>
+    <tableColumn id="148" xr3:uid="{00000000-0010-0000-0000-000094000000}" name="Where did the research take place/what is the location of the reference?11" dataDxfId="9"/>
+    <tableColumn id="149" xr3:uid="{00000000-0010-0000-0000-000095000000}" name="Reference description9" dataDxfId="8"/>
+    <tableColumn id="150" xr3:uid="{00000000-0010-0000-0000-000096000000}" name="Cover and/or forest type11" dataDxfId="7"/>
+    <tableColumn id="151" xr3:uid="{00000000-0010-0000-0000-000097000000}" name="Stable URL or DOI11" dataDxfId="6"/>
+    <tableColumn id="152" xr3:uid="{00000000-0010-0000-0000-000098000000}" name="Place published5" dataDxfId="5"/>
+    <tableColumn id="153" xr3:uid="{00000000-0010-0000-0000-000099000000}" name="Publisher5" dataDxfId="4"/>
+    <tableColumn id="154" xr3:uid="{00000000-0010-0000-0000-00009A000000}" name="Page Range4" dataDxfId="3"/>
+    <tableColumn id="155" xr3:uid="{00000000-0010-0000-0000-00009B000000}" name="Volume6" dataDxfId="2"/>
+    <tableColumn id="156" xr3:uid="{00000000-0010-0000-0000-00009C000000}" name="Edition5" dataDxfId="1"/>
+    <tableColumn id="157" xr3:uid="{00000000-0010-0000-0000-00009D000000}" name="Section" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2872,19 +2875,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FA13"/>
+  <dimension ref="A1:FA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="157" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="158" max="16384" width="9.140625" style="2"/>
+    <col min="158" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3357,7 +3360,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A2" s="2">
         <v>15</v>
       </c>
@@ -3552,7 +3555,7 @@
       <c r="EZ2" s="1"/>
       <c r="FA2" s="1"/>
     </row>
-    <row r="3" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A3" s="2">
         <v>16</v>
       </c>
@@ -3743,7 +3746,7 @@
       <c r="EZ3" s="1"/>
       <c r="FA3" s="1"/>
     </row>
-    <row r="4" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A4" s="2">
         <v>17</v>
       </c>
@@ -3938,7 +3941,7 @@
       <c r="EZ4" s="1"/>
       <c r="FA4" s="1"/>
     </row>
-    <row r="5" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A5" s="2">
         <v>21</v>
       </c>
@@ -4135,7 +4138,7 @@
       <c r="EZ5" s="1"/>
       <c r="FA5" s="1"/>
     </row>
-    <row r="6" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A6" s="2">
         <v>22</v>
       </c>
@@ -4330,7 +4333,7 @@
       <c r="EZ6" s="1"/>
       <c r="FA6" s="1"/>
     </row>
-    <row r="7" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A7" s="2">
         <v>29</v>
       </c>
@@ -4519,7 +4522,7 @@
       <c r="EZ7" s="1"/>
       <c r="FA7" s="1"/>
     </row>
-    <row r="8" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A8" s="2">
         <v>53</v>
       </c>
@@ -4576,7 +4579,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A9" s="2">
         <v>54</v>
       </c>
@@ -4642,7 +4645,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A10" s="2">
         <v>59</v>
       </c>
@@ -4690,7 +4693,7 @@
       </c>
       <c r="AA10" s="4"/>
     </row>
-    <row r="11" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A11" s="2">
         <v>60</v>
       </c>
@@ -4729,7 +4732,7 @@
       </c>
       <c r="AA11" s="4"/>
     </row>
-    <row r="12" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A12" s="2">
         <v>61</v>
       </c>
@@ -4768,7 +4771,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="13" spans="1:157" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:157" x14ac:dyDescent="0.75">
       <c r="A13" s="2">
         <v>63</v>
       </c>
@@ -4812,6 +4815,45 @@
       <c r="BV13" s="2" t="s">
         <v>291</v>
       </c>
+    </row>
+    <row r="14" spans="1:157" x14ac:dyDescent="0.75">
+      <c r="A14" s="2">
+        <v>60</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44882.385162036997</v>
+      </c>
+      <c r="C14" s="3">
+        <v>44882.387731481504</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="AA14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>